<commit_message>
changed scraper script to get revenue from each org
</commit_message>
<xml_diff>
--- a/guidestar/data/ID_data.xlsx
+++ b/guidestar/data/ID_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3d5802c32daedcc/Documents/Repositories/NLP Charity Research/guidestar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_D51EEC781B57865F6F5768F44E279EF944601CFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F7C1AD-F871-46A8-91EA-7E743889EA74}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_D51EEC781B57865F6F5768F44E279EF944601CFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34A5B16A-A7EE-43D3-92E0-2111E873B714}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>EIN</t>
   </si>
@@ -49,7 +49,10 @@
     <t>NTEE Code</t>
   </si>
   <si>
-    <t>Mission</t>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Mission Statement</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,10 +441,10 @@
     <col min="7" max="7" width="38.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="87.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,6 +474,9 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>